<commit_message>
dabbling with colored output, simplify &str params
Use `<S: Into<String>>` in most places that took a `&str` so that it
doesn't matter if the caller has a `&str` or a `String`
</commit_message>
<xml_diff>
--- a/playground/test.xlsx
+++ b/playground/test.xlsx
@@ -14,31 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="9">
-  <si>
-    <t>some</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>stuff</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>below</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>some</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>stuff</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>below</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>some</t>
     <phoneticPr fontId="1"/>
@@ -82,15 +58,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -277,18 +248,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -356,95 +330,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1">
         <f>(sum(A2:A21) * 5)</f>
-        <v>18</v>
+        <v/>
       </c>
       <c r="B1">
         <f>(sum(B2:B21) * 1000)</f>
-        <v>28</v>
+        <v/>
       </c>
       <c r="C1">
         <f>(sum(C2:C21) / 3.14)</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C9">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="2" spans="1:3"/>
+    <row r="3" spans="1:3"/>
+    <row r="4" spans="1:3"/>
+    <row r="5" spans="1:3"/>
+    <row r="6" spans="1:3"/>
+    <row r="7" spans="1:3"/>
+    <row r="8" spans="1:3"/>
+    <row r="9" spans="1:3"/>
     <row r="10" spans="1:3"/>
     <row r="11" spans="1:3"/>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="12" spans="1:3"/>
     <row r="13" spans="1:3"/>
     <row r="14" spans="1:3"/>
     <row r="15" spans="1:3"/>
@@ -456,13 +368,13 @@
     <row r="21" spans="1:3"/>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>